<commit_message>
send message, admin filter added
</commit_message>
<xml_diff>
--- a/Task to do.xlsx
+++ b/Task to do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manik\Documents\Live Projects\mBlogLive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1176F4F-BE60-49DC-A622-E52C389E79E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C3422B-0749-49FB-829C-C2D912F83795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>S.No</t>
   </si>
@@ -34,6 +34,12 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -85,10 +91,16 @@
     <t>Send Message form</t>
   </si>
   <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
+    <t>17-07-2025</t>
+  </si>
+  <si>
+    <t>Django Admin Filters</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>This is for wright for us, send message, subscribers.</t>
   </si>
 </sst>
 </file>
@@ -138,32 +150,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -175,6 +172,21 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -184,12 +196,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -198,20 +231,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,375 +545,390 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.21875" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6">
+        <v>45852</v>
+      </c>
+      <c r="F2" s="6">
+        <v>45852</v>
+      </c>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="C10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="9">
-        <v>45852</v>
-      </c>
-      <c r="F2" s="9">
-        <v>45852</v>
-      </c>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="E11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="B12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="D12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
forms and messages completed
</commit_message>
<xml_diff>
--- a/Task to do.xlsx
+++ b/Task to do.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>S.No</t>
   </si>
@@ -82,6 +82,9 @@
     <t>Subcriber Newletter form</t>
   </si>
   <si>
+    <t>19-07-2025</t>
+  </si>
+  <si>
     <t>Send Message form</t>
   </si>
   <si>
@@ -95,6 +98,9 @@
   </si>
   <si>
     <t>This is for wright for us, send message, subscribers.</t>
+  </si>
+  <si>
+    <t>Messages fine tune for all form</t>
   </si>
 </sst>
 </file>
@@ -739,10 +745,14 @@
         <v>8</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+        <v>9</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="G10" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
@@ -750,7 +760,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>8</v>
@@ -759,10 +769,10 @@
         <v>9</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G11" s="8"/>
     </row>
@@ -771,7 +781,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>8</v>
@@ -780,22 +790,34 @@
         <v>9</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G12" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="F13" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="G13" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
@@ -816,7 +838,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>

</xml_diff>

<commit_message>
news and snippet completed
</commit_message>
<xml_diff>
--- a/Task to do.xlsx
+++ b/Task to do.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
   <si>
     <t>S.No</t>
   </si>
@@ -52,12 +52,15 @@
     <t>Medium</t>
   </si>
   <si>
+    <t>20-07-2025</t>
+  </si>
+  <si>
+    <t>Tools</t>
+  </si>
+  <si>
     <t>Not Started</t>
   </si>
   <si>
-    <t>Tools</t>
-  </si>
-  <si>
     <t>DRF implementaions</t>
   </si>
   <si>
@@ -101,6 +104,12 @@
   </si>
   <si>
     <t>Messages fine tune for all form</t>
+  </si>
+  <si>
+    <t>Env for development server</t>
+  </si>
+  <si>
+    <t>High</t>
   </si>
 </sst>
 </file>
@@ -142,7 +151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -193,11 +202,18 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -224,6 +240,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -546,13 +565,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="7.147857142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="32.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="7.147857142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="13" width="23.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -578,7 +597,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -609,11 +628,15 @@
       <c r="C3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="F3" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="G3" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
@@ -626,8 +649,8 @@
       <c r="C4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>12</v>
+      <c r="D4" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -638,7 +661,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>8</v>
@@ -647,10 +670,10 @@
         <v>9</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5" s="8"/>
     </row>
@@ -659,7 +682,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>8</v>
@@ -668,10 +691,10 @@
         <v>9</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G6" s="8"/>
     </row>
@@ -680,16 +703,20 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="F7" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="G7" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -697,7 +724,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>8</v>
@@ -706,10 +733,10 @@
         <v>9</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G8" s="8"/>
     </row>
@@ -718,7 +745,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>8</v>
@@ -727,10 +754,10 @@
         <v>9</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G9" s="8"/>
     </row>
@@ -739,7 +766,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>8</v>
@@ -748,10 +775,10 @@
         <v>9</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G10" s="8"/>
     </row>
@@ -760,7 +787,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>8</v>
@@ -769,10 +796,10 @@
         <v>9</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G11" s="8"/>
     </row>
@@ -781,7 +808,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>8</v>
@@ -790,13 +817,13 @@
         <v>9</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="10" t="s">
         <v>27</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -804,7 +831,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>11</v>
@@ -813,18 +840,26 @@
         <v>9</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G13" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="8"/>

</xml_diff>

<commit_message>
Author page setup done
</commit_message>
<xml_diff>
--- a/Task to do.xlsx
+++ b/Task to do.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
   <si>
     <t>S.No</t>
   </si>
@@ -116,6 +116,21 @@
   </si>
   <si>
     <t>News page fintune</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>21-07-2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author page </t>
+  </si>
+  <si>
+    <t>23-07-2025</t>
+  </si>
+  <si>
+    <t>Sitemap update</t>
   </si>
 </sst>
 </file>
@@ -898,28 +913,54 @@
         <v>31</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="9"/>
+        <v>34</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="F16" s="9"/>
       <c r="G16" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="G17" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="G18" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
@@ -958,7 +999,7 @@
       <c r="F22" s="9"/>
       <c r="G22" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>

</xml_diff>